<commit_message>
Added regression report for version DanpheEMMR_V1.48.9 updated system library file
</commit_message>
<xml_diff>
--- a/SystemTest/SystemTestCases.xlsx
+++ b/SystemTest/SystemTestCases.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\svn\DanpheEMR\SystemTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\SystemTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="124">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -195,9 +195,6 @@
     <t>TC031</t>
   </si>
   <si>
-    <t>Inventory\Reports\TC001CreateGoodReceipt.py</t>
-  </si>
-  <si>
     <t>TC032</t>
   </si>
   <si>
@@ -381,19 +378,25 @@
     <t>Inventory\Reports\TC002CurrentStockLevelReport.py</t>
   </si>
   <si>
-    <t>TC</t>
-  </si>
-  <si>
     <t>Scripting Status</t>
   </si>
   <si>
     <t>Inventory\Reports\TC003 InventorySummaryReport.py</t>
+  </si>
+  <si>
+    <t>TC056</t>
+  </si>
+  <si>
+    <t>TC057</t>
+  </si>
+  <si>
+    <t>Inventory\TC001CreateGoodReceipt.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +773,7 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -787,19 +790,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -864,7 +867,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -884,7 +887,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
@@ -904,7 +907,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -924,7 +927,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
@@ -944,7 +947,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
@@ -964,7 +967,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
@@ -984,7 +987,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
@@ -1004,7 +1007,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>9</v>
@@ -1024,7 +1027,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -1424,19 +1427,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>9</v>
@@ -1456,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1464,7 +1467,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>9</v>
@@ -1476,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1484,7 +1487,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>9</v>
@@ -1496,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1504,7 +1507,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>9</v>
@@ -1516,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1524,7 +1527,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>9</v>
@@ -1536,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1544,7 +1547,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>9</v>
@@ -1556,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -1564,7 +1567,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>9</v>
@@ -1576,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1584,7 +1587,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>9</v>
@@ -1596,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1604,7 +1607,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>9</v>
@@ -1616,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -1624,7 +1627,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>9</v>
@@ -1636,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1644,7 +1647,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>9</v>
@@ -1656,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -1664,7 +1667,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>9</v>
@@ -1676,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -1684,7 +1687,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>9</v>
@@ -1696,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1704,7 +1707,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>9</v>
@@ -1716,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1724,7 +1727,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>9</v>
@@ -1736,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -1744,7 +1747,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>9</v>
@@ -1756,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1764,7 +1767,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>9</v>
@@ -1776,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -1784,7 +1787,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>9</v>
@@ -1796,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1804,7 +1807,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>9</v>
@@ -1816,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -1824,7 +1827,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>9</v>
@@ -1836,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -1844,7 +1847,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>9</v>
@@ -1856,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -1864,7 +1867,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>9</v>
@@ -1876,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -1884,7 +1887,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>9</v>
@@ -1896,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -1904,7 +1907,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>9</v>
@@ -1916,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -1924,7 +1927,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>9</v>
@@ -1936,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>

</xml_diff>

<commit_message>
changes in multiple files (Automation update V2.0)
</commit_message>
<xml_diff>
--- a/SystemTest/SystemTestCases.xlsx
+++ b/SystemTest/SystemTestCases.xlsx
@@ -303,9 +303,6 @@
     <t>Billing\OPbilling\TC009CreateProvisionalBill.py</t>
   </si>
   <si>
-    <t>Billing\OPbilling\TC010CancelIPProvisionalBill.py</t>
-  </si>
-  <si>
     <t>Billing\OPbilling\TC011CreateCopyOfItemsCashInvoice.py</t>
   </si>
   <si>
@@ -391,6 +388,9 @@
   </si>
   <si>
     <t>Inventory\TC001CreateGoodReceipt.py</t>
+  </si>
+  <si>
+    <t>Billing\IPbilling\TC010CancelIPProvisionalBill.py</t>
   </si>
 </sst>
 </file>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,10 +790,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>83</v>
@@ -802,7 +802,7 @@
         <v>85</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>9</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>9</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>9</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>9</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>9</v>
@@ -1759,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>9</v>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>9</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>9</v>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>9</v>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>9</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>9</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>9</v>
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>9</v>
@@ -1919,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>9</v>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>

</xml_diff>